<commit_message>
Added Mid-Game attacks in the .md file and in our game
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/pmSheet.xlsx
+++ b/01_ProjectPlanning/pmSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO\Desktop\HTL\Programmieren\Project\if.05.61_01-project-repository\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E443AF-6083-4D27-A434-B872CAB09985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00A8D01-A00D-4EA8-A958-CB41B0594831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F780517-EDF3-40DE-9578-A00B65031757}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,14 +508,14 @@
         <v>15</v>
       </c>
       <c r="C3" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
         <v>4</v>
       </c>
       <c r="E3" s="1">
         <f>C3-D3</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -529,14 +529,14 @@
         <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ref="E4:E23" si="0">C4-D4</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -571,14 +571,14 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -661,11 +661,11 @@
         <v>6</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
@@ -682,11 +682,11 @@
         <v>15</v>
       </c>
       <c r="D14" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Finished all attacks (excluded Combo and Soulbar attacks)
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/pmSheet.xlsx
+++ b/01_ProjectPlanning/pmSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO\Desktop\HTL\Programmieren\Project\if.05.61_01-project-repository\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00A8D01-A00D-4EA8-A958-CB41B0594831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF1497F-02F6-4672-BE0B-D8CAD9903088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F780517-EDF3-40DE-9578-A00B65031757}"/>
   </bookViews>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7A473B-8019-4D26-B2B4-6F04769690C4}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,11 +682,11 @@
         <v>15</v>
       </c>
       <c r="D14" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>

</xml_diff>